<commit_message>
fixing the large file problem.
</commit_message>
<xml_diff>
--- a/Project 2 - Transportation/Main Project/Anaheim.xlsx
+++ b/Project 2 - Transportation/Main Project/Anaheim.xlsx
@@ -477,37 +477,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.1416479967586096</v>
+        <v>0.1314760660418569</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1676145534843051</v>
+        <v>0.1539913361597004</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1816056544610492</v>
+        <v>0.1565234345817243</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1717796738427407</v>
+        <v>0.1551905170381066</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1806938988889073</v>
+        <v>0.1617439180799539</v>
       </c>
       <c r="G2" t="n">
-        <v>0.197875053086659</v>
+        <v>0.1682780233288715</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1686171467547355</v>
+        <v>0.1663779121061461</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1710028606501674</v>
+        <v>0.1651519145690534</v>
       </c>
       <c r="J2" t="n">
-        <v>0.1442706395381127</v>
+        <v>0.1902265616939454</v>
       </c>
       <c r="K2" t="n">
-        <v>0.161649701817723</v>
+        <v>0.2377974956836507</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1455050767778137</v>
+        <v>0.2665114867765981</v>
       </c>
     </row>
     <row r="3">
@@ -547,7 +547,7 @@
         <v>0.2347972943644358</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1354230858627253</v>
+        <v>0.2652356755644795</v>
       </c>
     </row>
     <row r="4">
@@ -557,37 +557,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0251474893</v>
+        <v>0.00069180586</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03233052</v>
+        <v>0.001120076733</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0310928879999999</v>
+        <v>0.001463898181</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0390645321</v>
+        <v>0.001599258038</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0405810655</v>
+        <v>0.0025209902609999</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0307912167</v>
+        <v>0.001747938681</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0527011181999999</v>
+        <v>0.002747082528</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0434748763999999</v>
+        <v>0.0020482382289999</v>
       </c>
       <c r="J4" t="n">
-        <v>0.09094375490000001</v>
+        <v>0.015178175733</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1323098892</v>
+        <v>0.0309456518799999</v>
       </c>
       <c r="L4" t="n">
-        <v>0.2445415487</v>
+        <v>0.08993521124999999</v>
       </c>
     </row>
     <row r="5">
@@ -669,37 +669,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0091767621677882</v>
+        <v>0.0079309986353268</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0126815816826207</v>
+        <v>0.0102146219988084</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0136023607909506</v>
+        <v>0.0103751151697287</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0126590446736734</v>
+        <v>0.0112233210163918</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0146245407375791</v>
+        <v>0.0116215710888588</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0186444497523609</v>
+        <v>0.0119180797612574</v>
       </c>
       <c r="H2" t="n">
-        <v>0.0149168806977097</v>
+        <v>0.0125446740228074</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0128486936133055</v>
+        <v>0.0119534396582186</v>
       </c>
       <c r="J2" t="n">
-        <v>0.0100663286175858</v>
+        <v>0.016104213883986</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0108986081853278</v>
+        <v>0.026233215683518</v>
       </c>
       <c r="L2" t="n">
-        <v>0.009664624952021099</v>
+        <v>0.0401903358813225</v>
       </c>
     </row>
     <row r="3">
@@ -739,7 +739,7 @@
         <v>0.0258957253123784</v>
       </c>
       <c r="L3" t="n">
-        <v>0.008395540314722</v>
+        <v>0.0397596732577202</v>
       </c>
     </row>
     <row r="4">
@@ -749,37 +749,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.01400673254</v>
+        <v>0.01265712069</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01779903835</v>
+        <v>0.0167630054</v>
       </c>
       <c r="D4" t="n">
-        <v>0.015058882</v>
+        <v>0.0188191312</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0221375878</v>
+        <v>0.0170885715999999</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0214828773</v>
+        <v>0.0216194767</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0163214785999999</v>
+        <v>0.0216247891999999</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0256711475</v>
+        <v>0.0223227046</v>
       </c>
       <c r="I4" t="n">
-        <v>0.0218387003</v>
+        <v>0.0204234979</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0479038442999999</v>
+        <v>0.0407220841999999</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0738470359</v>
+        <v>0.08704592680000001</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1137946938</v>
+        <v>0.1112948892</v>
       </c>
     </row>
     <row r="5">
@@ -861,37 +861,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9129381666302951</v>
+        <v>0.9173913742568482</v>
       </c>
       <c r="C2" t="n">
-        <v>0.942371354990188</v>
+        <v>0.9044129292452292</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9305682719614417</v>
+        <v>0.917552372541501</v>
       </c>
       <c r="E2" t="n">
-        <v>0.909880230529848</v>
+        <v>0.8924757867843361</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9169333199535132</v>
+        <v>0.9251649293266334</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9266494327330904</v>
+        <v>0.9261842502552058</v>
       </c>
       <c r="H2" t="n">
-        <v>0.913186313970062</v>
+        <v>0.9378839388229336</v>
       </c>
       <c r="I2" t="n">
-        <v>0.907221404285442</v>
+        <v>0.917691965884882</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9020890167424612</v>
+        <v>0.9267723812437452</v>
       </c>
       <c r="K2" t="n">
-        <v>0.8993068969704447</v>
+        <v>0.8956144804054714</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9098822342552816</v>
+        <v>0.9190230818393684</v>
       </c>
     </row>
     <row r="3">
@@ -931,7 +931,7 @@
         <v>0.9018502063939746</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9163697822918886</v>
+        <v>0.920940536058258</v>
       </c>
     </row>
     <row r="4">
@@ -941,37 +941,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8590496517597052</v>
+        <v>0.8693940760788929</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8162351847136391</v>
+        <v>0.8564086219995067</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8937600228899129</v>
+        <v>0.8660991237146579</v>
       </c>
       <c r="E4" t="n">
-        <v>0.787637525197991</v>
+        <v>0.7995486822420237</v>
       </c>
       <c r="F4" t="n">
-        <v>0.814725068597569</v>
+        <v>0.8619152368481243</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9308927476872708</v>
+        <v>0.8809842592885347</v>
       </c>
       <c r="H4" t="n">
-        <v>0.7944798042038623</v>
+        <v>0.8659263772821619</v>
       </c>
       <c r="I4" t="n">
-        <v>0.7894852998925626</v>
+        <v>0.8253791510425946</v>
       </c>
       <c r="J4" t="n">
-        <v>0.7114011971523049</v>
+        <v>0.805359012312356</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5747396804833298</v>
+        <v>0.4648407514572487</v>
       </c>
       <c r="L4" t="n">
-        <v>0.383700770414617</v>
+        <v>0.0046772373742857</v>
       </c>
     </row>
     <row r="5">

</xml_diff>